<commit_message>
adicionado arquivos originais e adicionado traducao das falas
algumas falam estavam em um arquivo corrompido, no qual eu ja resolvi

o arquivo corrompido era do jogo, e nao da traducao
</commit_message>
<xml_diff>
--- a/PTBR/Lang/PTBR/Game/Religion.xlsx
+++ b/PTBR/Lang/PTBR/Game/Religion.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isy\Documents\GitHub\elin-portugues-brasileiro\Traduzido\PTBR\Lang\PTBR\Game\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\SteamLibrary\steamapps\common\Elin\Package\PTBR\Lang\PTBR\Game\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F440BC9-44F5-4374-B576-E4CF8BF2EBBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9888FFE9-B8A6-4408-BF46-8B8581981A59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="165" yWindow="225" windowWidth="13125" windowHeight="14670" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Religion" sheetId="1" r:id="rId1"/>
@@ -993,9 +993,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
+      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>